<commit_message>
creato modulo per certificates
</commit_message>
<xml_diff>
--- a/output/import.xlsx
+++ b/output/import.xlsx
@@ -4,11 +4,10 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Output" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -45,15 +44,83 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -346,24 +413,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:BG24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1519,6 +1568,11 @@
       </c>
     </row>
     <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>BNP Paribas Issuance B.V.</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>NL0014919474</t>
@@ -1534,6 +1588,11 @@
           <t>FR0010613471</t>
         </is>
       </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>26 May 2020.</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr">
         <is>
           <t>26/05/20
@@ -1546,8 +1605,18 @@
       <c r="R21" t="n">
         <v>100</v>
       </c>
+      <c r="AN21" t="inlineStr">
+        <is>
+          <t>The settlement currency for the payment of the Cash Settlement Amount is Euro ("EUR")</t>
+        </is>
+      </c>
     </row>
     <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BNP Paribas Issuance B.V.</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
           <t>NL0014919474</t>
@@ -1563,6 +1632,11 @@
           <t>FR0000124141</t>
         </is>
       </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>26 May 2020.</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr">
         <is>
           <t>26/05/20
@@ -1575,8 +1649,18 @@
       <c r="R22" t="n">
         <v>100</v>
       </c>
+      <c r="AN22" t="inlineStr">
+        <is>
+          <t>The settlement currency for the payment of the Cash Settlement Amount is Euro ("EUR")</t>
+        </is>
+      </c>
     </row>
     <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>BNP Paribas Issuance B.V.</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>NL0014919482</t>
@@ -1592,6 +1676,11 @@
           <t>IT0003132476</t>
         </is>
       </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>26 May 2020.</t>
+        </is>
+      </c>
       <c r="I23" t="inlineStr">
         <is>
           <t>26/05/20
@@ -1604,8 +1693,18 @@
       <c r="R23" t="n">
         <v>100</v>
       </c>
+      <c r="AN23" t="inlineStr">
+        <is>
+          <t>The settlement currency for the payment of the Cash Settlement Amount is Euro ("EUR")</t>
+        </is>
+      </c>
     </row>
     <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>BNP Paribas Issuance B.V.</t>
+        </is>
+      </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>NL0014919482</t>
@@ -1621,6 +1720,11 @@
           <t>FR0000120271</t>
         </is>
       </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>26 May 2020.</t>
+        </is>
+      </c>
       <c r="I24" t="inlineStr">
         <is>
           <t>26/05/20
@@ -1633,8 +1737,13 @@
       <c r="R24" t="n">
         <v>100</v>
       </c>
+      <c r="AN24" t="inlineStr">
+        <is>
+          <t>The settlement currency for the payment of the Cash Settlement Amount is Euro ("EUR")</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>